<commit_message>
develop afo input params
</commit_message>
<xml_diff>
--- a/public/eco_refs_analysis_param.xlsx
+++ b/public/eco_refs_analysis_param.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Месяц</t>
   </si>
@@ -86,7 +86,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.0\ _₽_-;\-* #,##0.0\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.0\ _₽_-;\-* #,##0.0\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -149,7 +149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -157,19 +157,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -451,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -463,136 +460,122 @@
     <col min="2" max="2" width="22.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="23.140625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="23.7109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="16.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="23.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>8</v>
-      </c>
-      <c r="B3" s="7">
+        <v>44197</v>
+      </c>
+      <c r="B3" s="5">
         <v>46381.292791617387</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>61179.098336085633</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <v>61179.098336085633</v>
       </c>
-      <c r="E3" s="7">
-        <v>61179.098336085633</v>
-      </c>
-      <c r="F3" s="7">
+      <c r="E3" s="5">
         <v>300.9030937194799</v>
       </c>
-      <c r="G3" s="7">
-        <f>K3/J3</f>
-        <v>65.55480333120174</v>
-      </c>
-      <c r="H3" s="7">
+      <c r="F3" s="5">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="G3" s="5">
         <v>1948</v>
       </c>
-      <c r="I3" s="7">
+      <c r="H3" s="5">
         <v>0.83899999999999997</v>
       </c>
-      <c r="J3" s="7">
+      <c r="I3" s="5">
         <v>31</v>
       </c>
-      <c r="K3" s="7">
+      <c r="J3" s="5">
         <v>2032.1989032672541</v>
       </c>
-      <c r="L3" s="7">
-        <f>G3*0.7</f>
-        <v>45.888362331841215</v>
-      </c>
-      <c r="M3" s="7">
+      <c r="K3" s="5">
+        <v>45.9</v>
+      </c>
+      <c r="L3" s="5">
         <v>45.888362331841215</v>
       </c>
     </row>

</xml_diff>